<commit_message>
Semi USB: checklist: Updating schematic section of spreedsheet, almost all points done #24
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/3_Interface_QuadUART/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/3_Interface_QuadUART/PCB Design Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\1_Interface_QuadUART\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\3_Interface_QuadUART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BC66D8-8E65-44AD-874B-6CA07DBC4D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95BC724-A78C-4F12-BC71-F2266F0F9C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3645" windowWidth="29040" windowHeight="15840" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="168">
   <si>
     <t>1.</t>
   </si>
@@ -473,9 +473,6 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>Project: Interface Board for FloripaSat-2</t>
-  </si>
-  <si>
     <t>Yan Castro de Azeredo</t>
   </si>
   <si>
@@ -485,13 +482,61 @@
     <t>Drawing</t>
   </si>
   <si>
-    <t>USB powered bus</t>
-  </si>
-  <si>
     <t>PCB Design Checklist by Kleber Reis Gouveia Júnior</t>
   </si>
   <si>
-    <t>Variant: Semi USB - Quad UART Interface 1º Board</t>
+    <t>Project: Interstage Interface Panels of FloripaSat-2</t>
+  </si>
+  <si>
+    <t>Variant: Semi USB - Quad UART Interface Board Nº3</t>
+  </si>
+  <si>
+    <t>USB 5V powered bus</t>
+  </si>
+  <si>
+    <t>Waiting some feedback</t>
+  </si>
+  <si>
+    <t>Opted for not using a shift register in project for simplification</t>
+  </si>
+  <si>
+    <t>Ceramic are more indicated</t>
+  </si>
+  <si>
+    <t>Opted for a more simple design</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>Add schematic template to project</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>Add block diagram of the project</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>Add info about project, drawer, reviewers and supporters</t>
+  </si>
+  <si>
+    <t>Waiting further feedback</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Elaborate PCB design rules for targeted manufacturer</t>
+  </si>
+  <si>
+    <t>Needs revision especialy the external EEPROM pins</t>
+  </si>
+  <si>
+    <t>Only picoblade polarity headers taked into account</t>
   </si>
 </sst>
 </file>
@@ -634,7 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -714,6 +759,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1033,10 +1084,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1100,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1059,7 +1110,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1067,13 +1118,13 @@
         <v>68</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1082,7 +1133,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43949.473164930554</v>
+        <v>44003.478417939812</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1129,7 +1180,7 @@
         <v>133</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1140,9 +1191,13 @@
         <v>78</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1153,8 +1208,12 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1164,9 +1223,13 @@
         <v>77</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1175,7 +1238,9 @@
       <c r="B10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="7"/>
@@ -1187,10 +1252,14 @@
       <c r="B11" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1200,7 +1269,9 @@
         <v>92</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="7"/>
     </row>
@@ -1213,8 +1284,12 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1223,7 +1298,9 @@
       <c r="B14" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="7"/>
@@ -1236,9 +1313,13 @@
         <v>91</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -1247,7 +1328,9 @@
       <c r="B16" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="7"/>
@@ -1259,7 +1342,9 @@
       <c r="B17" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="7"/>
@@ -1271,7 +1356,9 @@
       <c r="B18" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="7"/>
@@ -1283,7 +1370,9 @@
       <c r="B19" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="7"/>
@@ -1297,8 +1386,12 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
@@ -1321,93 +1414,105 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>66</v>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1416,10 +1521,10 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1428,10 +1533,10 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1440,10 +1545,10 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1452,10 +1557,10 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1464,10 +1569,10 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1476,10 +1581,10 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1488,10 +1593,10 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1500,10 +1605,10 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1512,10 +1617,10 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1524,10 +1629,10 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1536,10 +1641,10 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1548,10 +1653,10 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1560,10 +1665,10 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1572,10 +1677,10 @@
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1584,10 +1689,10 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1596,10 +1701,10 @@
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1608,10 +1713,10 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1620,10 +1725,10 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1632,10 +1737,10 @@
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1644,10 +1749,10 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1656,10 +1761,10 @@
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1668,10 +1773,10 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1680,10 +1785,10 @@
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1692,10 +1797,10 @@
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1704,10 +1809,10 @@
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -1716,10 +1821,10 @@
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1728,10 +1833,10 @@
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1740,10 +1845,10 @@
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -1752,10 +1857,10 @@
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -1764,10 +1869,10 @@
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1776,100 +1881,100 @@
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B61" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>66</v>
-      </c>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>137</v>
+        <v>52</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="C63" s="2"/>
-      <c r="D63" s="1"/>
+      <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>138</v>
+        <v>53</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="C64" s="2"/>
-      <c r="D64" s="1"/>
+      <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="24"/>
+      <c r="C66" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="1"/>
@@ -1878,10 +1983,10 @@
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="1"/>
@@ -1890,10 +1995,10 @@
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="1"/>
@@ -1902,10 +2007,10 @@
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="1"/>
@@ -1914,93 +2019,141 @@
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="1"/>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B76" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="25" t="s">
+      <c r="B77" s="23"/>
+      <c r="C77" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D73" s="26"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="16" t="s">
+      <c r="D77" s="26"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B74" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="14"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+      <c r="B78" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="14"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="14"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="14"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="14"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C77:E77"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>